<commit_message>
Add Find element for login validation
</commit_message>
<xml_diff>
--- a/Academy-REF-Acme-CalculateClientSecurityHash/Data/Config.xlsx
+++ b/Academy-REF-Acme-CalculateClientSecurityHash/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denni\Documents\UiPath\Academy-REF-Acme-CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316A3C6A-5712-4707-95C1-55341AFAD077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61922728-3FF1-4488-9E0B-F447A0B2EC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1664,15 +1664,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
     <col min="3" max="3" width="75.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
@@ -2818,7 +2818,6 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>